<commit_message>
1. Test cases updated (added new for create/modify/remove)
</commit_message>
<xml_diff>
--- a/test cases/TC KanbanBoard.xlsx
+++ b/test cases/TC KanbanBoard.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
   <si>
     <t>Priority</t>
   </si>
@@ -238,19 +238,61 @@
   </si>
   <si>
     <t>1.Log in to KanbanBoard application
-2.Verify that 'Create' button is displayed and is active
-3.Click on 'Create' button
-4.Enter name of new board into 'title' field
-5.Click on 'Cancel' button
-6.Click on 'Create' button and enter name of new board
-7.Click on 'Create' button</t>
+2.Hover over a board 
+3.Click on 'Modify' icon
+4.Enter new name of the board and click on 'Cancel' button
+5.Hover over a board and click on 'Modify' icon
+6.Enter new name of the board and click 'Modify'
+7.Hover over a board and click on 'Modify' icon
+8.Enter new name of the board and click 'Enter' key</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.'Modify', 'Remove' icons are displayed
+3.Title of the 'board' become editable
+4.Title of the 'board' hasn't changed
+6.Title of the 'board' has changed
+8.Title of the 'board' has changed
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.Log in to KanbanBoard application
+2.Hover over a board 
+3.Click on 'Remove' icon
+4.In confirmation dialog click on 'No' button
+5.Hover over a board and click on 'Remove' icon
+6.In confirmation dialog click on 'Yes' button
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.'Modify', 'Remove' icons are displayed
+3.Confirmation dialog appears
+4.Board has not been removed
+5.Board has been removed
+</t>
+  </si>
+  <si>
+    <t>1.Log in to KanbanBoard application
+2.Click on 'Create' button
+3.Enter name of new board into 'title' field
+4.Click on 'Cancel' button
+5.Click on 'Create' button and enter name of new board
+6.Click on 'Create' button</t>
+  </si>
+  <si>
+    <t>1.'Create' button is displayed and is active
+2.New dialog is displayed
+4.Board is not created and not is displayed
+6.Board is created and displayed in the board's list</t>
+  </si>
+  <si>
+    <t>verify board in DB</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -297,8 +339,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -322,8 +372,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -359,12 +414,28 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -405,9 +476,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="2" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Input" xfId="2" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -709,8 +784,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -975,7 +1050,7 @@
       <c r="Q6" s="13"/>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="114.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>7</v>
       </c>
@@ -993,12 +1068,16 @@
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="J7" s="10"/>
-      <c r="K7" s="3"/>
+      <c r="K7" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="L7" s="3"/>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
@@ -1007,7 +1086,7 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="165.75" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>7</v>
       </c>
@@ -1024,11 +1103,17 @@
         <v>50</v>
       </c>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>56</v>
+      </c>
       <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>57</v>
+      </c>
       <c r="J8" s="10"/>
-      <c r="K8" s="3"/>
+      <c r="K8" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="L8" s="3"/>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1037,7 +1122,7 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="102" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>7</v>
       </c>
@@ -1054,11 +1139,17 @@
         <v>51</v>
       </c>
       <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="J9" s="10"/>
-      <c r="K9" s="3"/>
+      <c r="K9" s="14" t="s">
+        <v>62</v>
+      </c>
       <c r="L9" s="3"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1068,9 +1159,13 @@
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A10" s="11"/>
+      <c r="A10" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
+      <c r="C10" s="3">
+        <v>9</v>
+      </c>
       <c r="D10" s="3"/>
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
@@ -1088,9 +1183,13 @@
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.2">
-      <c r="A11" s="11"/>
+      <c r="A11" s="11" t="s">
+        <v>7</v>
+      </c>
       <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
       <c r="D11" s="3"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>

</xml_diff>

<commit_message>
Test cases (Sprint 1 tab) executed
</commit_message>
<xml_diff>
--- a/test cases/TC KanbanBoard.xlsx
+++ b/test cases/TC KanbanBoard.xlsx
@@ -4,20 +4,24 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="180" windowWidth="15180" windowHeight="7695"/>
+    <workbookView xWindow="120" yWindow="180" windowWidth="15180" windowHeight="7695" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BASE" sheetId="1" r:id="rId1"/>
+    <sheet name="Sprint 1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sprint 2" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">BASE!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Sprint 1'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint 2'!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="67">
   <si>
     <t>Priority</t>
   </si>
@@ -96,11 +100,6 @@
   <si>
     <t>2.Administrator login = 'admin'
 3.Administrator psw = 'admin'</t>
-  </si>
-  <si>
-    <t>4a.'Administration' page appears.
-4b.Only one tab 'Administration' is displayed. 
-4c.'User name' is displayed next to inscription 'Logged user'</t>
   </si>
   <si>
     <t>Preconditions</t>
@@ -287,12 +286,29 @@
   <si>
     <t>verify board in DB</t>
   </si>
+  <si>
+    <t>specified test data was skipped</t>
+  </si>
+  <si>
+    <t>2.Administrator login = 'admin'
+3.Administrator psw = '1'</t>
+  </si>
+  <si>
+    <t>4a.'Administration' page appears.
+4b.'User name' is displayed at the top right corner</t>
+  </si>
+  <si>
+    <t>for now it's possible to perform only first 4 steps</t>
+  </si>
+  <si>
+    <t>SSMK-42 - Application doesn't store user state (logged in / out)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,8 +363,33 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,6 +416,21 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
       </patternFill>
     </fill>
   </fills>
@@ -430,12 +486,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -479,10 +538,25 @@
     <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="3" xfId="5" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="6">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="5" builtinId="22"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Input" xfId="2" builtinId="20"/>
+    <cellStyle name="Neutral" xfId="4" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -784,8 +858,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -823,13 +897,13 @@
         <v>18</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I1" s="4" t="s">
         <v>6</v>
@@ -874,11 +948,11 @@
       </c>
       <c r="F2" s="8"/>
       <c r="G2" s="8" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H2" s="8"/>
       <c r="I2" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="10"/>
       <c r="K2" s="8"/>
@@ -907,20 +981,20 @@
         <v>2</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="H3" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="I3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="J3" s="10"/>
       <c r="K3" s="3"/>
@@ -938,7 +1012,7 @@
       </c>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="63.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -952,17 +1026,17 @@
         <v>24</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>25</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>26</v>
+        <v>64</v>
       </c>
       <c r="J4" s="10"/>
       <c r="K4" s="3"/>
@@ -985,24 +1059,24 @@
         <v>7</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C5" s="8">
         <v>4</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>40</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="H5" s="3"/>
       <c r="I5" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="J5" s="10"/>
       <c r="K5" s="5"/>
@@ -1021,24 +1095,24 @@
         <v>7</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3">
         <v>5</v>
       </c>
       <c r="D6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>42</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="H6" s="3"/>
       <c r="I6" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J6" s="10"/>
       <c r="K6" s="3"/>
@@ -1055,28 +1129,28 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C7" s="3">
         <v>6</v>
       </c>
       <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="H7" s="3"/>
       <c r="I7" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J7" s="10"/>
       <c r="K7" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="1"/>
@@ -1091,28 +1165,28 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" s="3">
         <v>7</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="H8" s="3"/>
       <c r="I8" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="J8" s="10"/>
       <c r="K8" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L8" s="3"/>
       <c r="M8" s="1"/>
@@ -1127,28 +1201,28 @@
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C9" s="3">
         <v>8</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="H9" s="3"/>
       <c r="I9" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="J9" s="10"/>
       <c r="K9" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="1"/>
@@ -1588,4 +1662,1646 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="2" customWidth="1"/>
+    <col min="4" max="6" width="23.140625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="39" style="2" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" ht="267.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="L3" s="3"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="K5" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="L5" s="3"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L6" s="3"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="K9" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L1"/>
+  <dataConsolidate/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L14">
+      <formula1>$P$3:$P$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J5:J14">
+      <formula1>$Q$3:$Q$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A4">
+      <formula1>$O$3:$O$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:R33"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="9" style="2" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" style="2" customWidth="1"/>
+    <col min="4" max="6" width="23.140625" style="2" customWidth="1"/>
+    <col min="7" max="8" width="39" style="2" customWidth="1"/>
+    <col min="9" max="9" width="30.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="10" style="2" customWidth="1"/>
+    <col min="11" max="11" width="22.7109375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" style="2" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" style="2"/>
+    <col min="15" max="15" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.140625" style="2" customWidth="1"/>
+    <col min="17" max="17" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="2"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="O1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="P1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R1" s="1"/>
+    </row>
+    <row r="2" spans="1:18" ht="76.5" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="8">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="8"/>
+      <c r="I2" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="J2" s="10"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="M2" s="1"/>
+      <c r="N2" s="1"/>
+      <c r="O2" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" s="1"/>
+    </row>
+    <row r="3" spans="1:18" ht="267.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="P3" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" spans="1:18" ht="51" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="10"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="P4" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R4" s="1"/>
+    </row>
+    <row r="5" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="8">
+        <v>4</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" s="3"/>
+      <c r="I5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="J5" s="10"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="3"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R5" s="1"/>
+    </row>
+    <row r="6" spans="1:18" ht="178.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J6" s="10"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="13"/>
+      <c r="P6" s="13"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" spans="1:18" ht="89.25" x14ac:dyDescent="0.2">
+      <c r="A7" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="3">
+        <v>6</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="J7" s="10"/>
+      <c r="K7" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" s="3"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+    </row>
+    <row r="8" spans="1:18" ht="165.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="3"/>
+      <c r="I8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="10"/>
+      <c r="K8" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L8" s="3"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+    </row>
+    <row r="9" spans="1:18" ht="102" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J9" s="10"/>
+      <c r="K9" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="L9" s="3"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+    </row>
+    <row r="10" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A10" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3">
+        <v>9</v>
+      </c>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+    </row>
+    <row r="11" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A11" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3">
+        <v>10</v>
+      </c>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+    </row>
+    <row r="12" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A12" s="11"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="10"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+    </row>
+    <row r="13" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A13" s="11"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="10"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+    </row>
+    <row r="14" spans="1:18" ht="15" x14ac:dyDescent="0.2">
+      <c r="A14" s="11"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="10"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="12"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1"/>
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A33" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L1"/>
+  <dataConsolidate/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A3:A4">
+      <formula1>$O$3:$O$5</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J4:J14">
+      <formula1>$Q$3:$Q$7</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="L3:L14">
+      <formula1>$P$3:$P$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>